<commit_message>
Fix some error in material 11
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/11 - 条件格式（高级）.xlsx
+++ b/Excel动手实验室 - 材料/11 - 条件格式（高级）.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\OfficeTraining\Excel动手实验室 - 材料\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18434" windowHeight="8097"/>
   </bookViews>
   <sheets>
     <sheet name="创建规则" sheetId="1" r:id="rId1"/>
@@ -167,14 +162,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -182,14 +177,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -198,7 +193,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -257,25 +252,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="强调文字颜色 5" xfId="1" builtinId="45"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -294,27 +282,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -381,7 +348,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,7 +383,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,7 +560,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -605,10 +572,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -793,7 +760,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -885,14 +852,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -978,10 +943,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>B2&gt;600000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>B2&gt;700000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -995,10 +960,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="26.375" customWidth="1"/>
-    <col min="3" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" customWidth="1"/>
+    <col min="3" max="4" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1174,12 +1139,12 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="containsBlanks" dxfId="3" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="containsErrors" dxfId="1" priority="1">
+    <cfRule type="containsErrors" dxfId="0" priority="1">
       <formula>ISERROR(D2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1195,11 +1160,11 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>